<commit_message>
Starting model with resnet crnn
</commit_message>
<xml_diff>
--- a/Writeups/Experiments.xlsx
+++ b/Writeups/Experiments.xlsx
@@ -9,12 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Fuzzy Boundary Exp" sheetId="1" r:id="rId1"/>
     <sheet name="Call Repeats Exp" sheetId="2" r:id="rId2"/>
-    <sheet name="Negative Factor Exp" sheetId="3" r:id="rId3"/>
+    <sheet name="Combined Number" sheetId="9" r:id="rId3"/>
+    <sheet name="Hierarchical Exp" sheetId="5" r:id="rId4"/>
+    <sheet name="Negative Factor Exp" sheetId="3" r:id="rId5"/>
+    <sheet name="Cuda SEED" sheetId="6" r:id="rId6"/>
+    <sheet name="Shift Window" sheetId="7" r:id="rId7"/>
+    <sheet name="No nn04d_20181030" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="56">
   <si>
     <t>Fuzzy Boundary</t>
   </si>
@@ -104,14 +109,115 @@
   </si>
   <si>
     <t>Call Repeats Test</t>
+  </si>
+  <si>
+    <t>With Validation F-score Selecting Criteria</t>
+  </si>
+  <si>
+    <t>Model_0</t>
+  </si>
+  <si>
+    <t>Model_1</t>
+  </si>
+  <si>
+    <t>Negative Factor Train Model 0</t>
+  </si>
+  <si>
+    <t>Negative Factor Test Model 0</t>
+  </si>
+  <si>
+    <t>Call Repeats Model 0</t>
+  </si>
+  <si>
+    <t>Adversarial Threshold</t>
+  </si>
+  <si>
+    <t>Call Repeats Model 1</t>
+  </si>
+  <si>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>CUDA</t>
+  </si>
+  <si>
+    <t>Model 0 P</t>
+  </si>
+  <si>
+    <t>Model 0 R</t>
+  </si>
+  <si>
+    <t>approx 33</t>
+  </si>
+  <si>
+    <t>aprox 91</t>
+  </si>
+  <si>
+    <t>Shift Window</t>
+  </si>
+  <si>
+    <t>FULL P With Sample</t>
+  </si>
+  <si>
+    <t>FULL R With Sample</t>
+  </si>
+  <si>
+    <t>Delta P</t>
+  </si>
+  <si>
+    <t>Delta R</t>
+  </si>
+  <si>
+    <t>Round2 P</t>
+  </si>
+  <si>
+    <t>Round2 R</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Round3 - old data init P</t>
+  </si>
+  <si>
+    <t>Round3 - old data init R</t>
+  </si>
+  <si>
+    <t>Round4 - No SEED P</t>
+  </si>
+  <si>
+    <t>Round4 - No SEED R</t>
+  </si>
+  <si>
+    <t>Round5 - SCHEDULAR P</t>
+  </si>
+  <si>
+    <t>Round4 - SCHEDULAR R</t>
+  </si>
+  <si>
+    <t>Round6 - SCHED + old data init P</t>
+  </si>
+  <si>
+    <t>Round6 - SCHED + old data init R</t>
+  </si>
+  <si>
+    <t>Subsample Data P/R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -134,8 +240,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,8 +271,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -172,23 +313,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2003,8 +2280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2126,115 +2403,115 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="20">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="b">
+      <c r="D4" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3">
-        <v>2</v>
-      </c>
-      <c r="I4" s="4">
+      <c r="E4" s="20">
+        <v>1</v>
+      </c>
+      <c r="F4" s="20">
+        <v>2</v>
+      </c>
+      <c r="G4" s="20">
+        <v>1</v>
+      </c>
+      <c r="H4" s="20">
+        <v>2</v>
+      </c>
+      <c r="I4" s="20">
         <v>27.4</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="20">
         <v>94.5</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3">
-        <v>5</v>
-      </c>
-      <c r="F5" s="3">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3">
-        <v>2</v>
-      </c>
-      <c r="I5" s="3">
+      <c r="B5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="20">
+        <v>5</v>
+      </c>
+      <c r="F5" s="20">
+        <v>2</v>
+      </c>
+      <c r="G5" s="20">
+        <v>1</v>
+      </c>
+      <c r="H5" s="20">
+        <v>2</v>
+      </c>
+      <c r="I5" s="20">
         <v>39.9</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="20">
         <v>90.3</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="20">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>5</v>
-      </c>
-      <c r="F6" s="3">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3">
+      <c r="D6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="20">
+        <v>5</v>
+      </c>
+      <c r="F6" s="20">
+        <v>2</v>
+      </c>
+      <c r="G6" s="20">
+        <v>1</v>
+      </c>
+      <c r="H6" s="20">
+        <v>2</v>
+      </c>
+      <c r="I6" s="20">
         <v>33.799999999999997</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="20">
         <v>92.2</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="3" t="b">
@@ -2296,13 +2573,13 @@
       <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>4</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="3" t="b">
@@ -2330,13 +2607,13 @@
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="3" t="b">
@@ -2364,7 +2641,7 @@
       <c r="L10" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I14" s="5"/>
+      <c r="I14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2374,10 +2651,392 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A2:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I12"/>
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="25"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8:I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="20">
+        <v>26.5</v>
+      </c>
+      <c r="I2" s="20">
+        <v>95.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>15</v>
+      </c>
+      <c r="H3" s="22">
+        <v>31</v>
+      </c>
+      <c r="I3" s="22">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>15</v>
+      </c>
+      <c r="H4" s="22">
+        <v>60.3</v>
+      </c>
+      <c r="I4" s="22">
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="5">
+        <v>15</v>
+      </c>
+      <c r="H5" s="22">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="I5" s="22">
+        <v>85.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="22">
+        <v>32.6</v>
+      </c>
+      <c r="I6" s="22">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5">
+        <v>15</v>
+      </c>
+      <c r="H7" s="20">
+        <v>56.3</v>
+      </c>
+      <c r="I7" s="20">
+        <v>83.4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>15</v>
+      </c>
+      <c r="H8" s="20">
+        <v>61.5</v>
+      </c>
+      <c r="I8" s="20">
+        <v>80.5</v>
+      </c>
+      <c r="J8">
+        <v>36.4</v>
+      </c>
+      <c r="K8">
+        <v>91.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>15</v>
+      </c>
+      <c r="H9" s="20">
+        <v>65.7</v>
+      </c>
+      <c r="I9" s="20">
+        <v>72.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3">
+        <v>17</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>5</v>
+      </c>
+      <c r="F10" s="5">
+        <v>2</v>
+      </c>
+      <c r="G10" s="5">
+        <v>15</v>
+      </c>
+      <c r="H10" s="23">
+        <v>53</v>
+      </c>
+      <c r="I10" s="23">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X33"/>
+  <sheetViews>
+    <sheetView zoomScale="98" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2389,9 +3048,14 @@
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="14" max="15" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.33203125" customWidth="1"/>
+    <col min="21" max="21" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2419,14 +3083,38 @@
       <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2448,14 +3136,47 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="13">
         <v>32.299999999999997</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="13">
         <v>93.7</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>32.6</v>
+      </c>
+      <c r="L2">
+        <v>92</v>
+      </c>
+      <c r="M2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2">
+        <v>30.2</v>
+      </c>
+      <c r="O2">
+        <v>90.8</v>
+      </c>
+      <c r="Q2">
+        <v>32.6</v>
+      </c>
+      <c r="R2">
+        <v>92</v>
+      </c>
+      <c r="T2">
+        <v>30.9</v>
+      </c>
+      <c r="U2">
+        <v>93.7</v>
+      </c>
+      <c r="W2">
+        <v>35.5</v>
+      </c>
+      <c r="X2">
+        <v>85.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2477,14 +3198,47 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="14">
         <v>33.700000000000003</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="14">
         <v>90.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>35.6</v>
+      </c>
+      <c r="L3">
+        <v>87</v>
+      </c>
+      <c r="M3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="O3">
+        <v>91.2</v>
+      </c>
+      <c r="Q3">
+        <v>35.6</v>
+      </c>
+      <c r="R3">
+        <v>87</v>
+      </c>
+      <c r="T3">
+        <v>30.7</v>
+      </c>
+      <c r="U3">
+        <v>92.9</v>
+      </c>
+      <c r="W3">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="X3">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2506,14 +3260,35 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="14">
         <v>33.200000000000003</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="14">
         <v>91.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>24.5</v>
+      </c>
+      <c r="L4">
+        <v>92.7</v>
+      </c>
+      <c r="M4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T4">
+        <v>33.6</v>
+      </c>
+      <c r="U4">
+        <v>88.7</v>
+      </c>
+      <c r="W4">
+        <v>33.6</v>
+      </c>
+      <c r="X4">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2535,14 +3310,24 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="14">
         <v>37.5</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="14">
         <v>86.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K5" s="34"/>
+      <c r="M5" t="s">
+        <v>46</v>
+      </c>
+      <c r="W5">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="X5">
+        <v>87.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2564,14 +3349,22 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="14">
         <v>36.9</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="14">
         <v>88.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2593,14 +3386,47 @@
       <c r="G8">
         <v>2</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="14">
         <v>26.5</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="14">
         <v>91.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>25.7</v>
+      </c>
+      <c r="L8">
+        <v>94.7</v>
+      </c>
+      <c r="M8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N8">
+        <v>32.6</v>
+      </c>
+      <c r="O8">
+        <v>94.3</v>
+      </c>
+      <c r="Q8">
+        <v>25.7</v>
+      </c>
+      <c r="R8">
+        <v>94.7</v>
+      </c>
+      <c r="T8">
+        <v>30.7</v>
+      </c>
+      <c r="U8">
+        <v>91.2</v>
+      </c>
+      <c r="W8">
+        <v>26.5</v>
+      </c>
+      <c r="X8">
+        <v>91.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2622,14 +3448,47 @@
       <c r="G9">
         <v>2</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="13">
         <v>39.9</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="13">
         <v>90.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>32.5</v>
+      </c>
+      <c r="L9">
+        <v>91.6</v>
+      </c>
+      <c r="M9" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9">
+        <v>33.9</v>
+      </c>
+      <c r="O9">
+        <v>89.4</v>
+      </c>
+      <c r="Q9">
+        <v>32.5</v>
+      </c>
+      <c r="R9">
+        <v>91.6</v>
+      </c>
+      <c r="T9">
+        <v>31.3</v>
+      </c>
+      <c r="U9">
+        <v>91.3</v>
+      </c>
+      <c r="W9">
+        <v>30.5</v>
+      </c>
+      <c r="X9">
+        <v>92.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2651,14 +3510,35 @@
       <c r="G10">
         <v>2</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="13">
         <v>48.4</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="13">
         <v>85.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <v>26.9</v>
+      </c>
+      <c r="L10">
+        <v>93.5</v>
+      </c>
+      <c r="M10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T10">
+        <v>35.4</v>
+      </c>
+      <c r="U10">
+        <v>89.9</v>
+      </c>
+      <c r="W10">
+        <v>48.4</v>
+      </c>
+      <c r="X10">
+        <v>85.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2680,14 +3560,14 @@
       <c r="G11">
         <v>2</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="14">
         <v>41</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="14">
         <v>85.7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2709,12 +3589,1180 @@
       <c r="G12">
         <v>2</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="14">
         <v>34.1</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="14">
         <v>90.3</v>
       </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="7">
+        <v>5</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8">
+        <v>4</v>
+      </c>
+      <c r="H14" s="15">
+        <v>30</v>
+      </c>
+      <c r="I14" s="15">
+        <v>92.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="7">
+        <v>5</v>
+      </c>
+      <c r="F15" s="7">
+        <v>2</v>
+      </c>
+      <c r="G15" s="8">
+        <v>4</v>
+      </c>
+      <c r="H15" s="15">
+        <v>31.6</v>
+      </c>
+      <c r="I15" s="15">
+        <v>92.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="7">
+        <v>5</v>
+      </c>
+      <c r="F16" s="7">
+        <v>5</v>
+      </c>
+      <c r="G16" s="8">
+        <v>4</v>
+      </c>
+      <c r="H16" s="12">
+        <v>36.1</v>
+      </c>
+      <c r="I16" s="12">
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="7">
+        <v>5</v>
+      </c>
+      <c r="F17" s="7">
+        <v>7</v>
+      </c>
+      <c r="G17" s="8">
+        <v>4</v>
+      </c>
+      <c r="H17" s="15">
+        <v>26.9</v>
+      </c>
+      <c r="I17" s="15">
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="7">
+        <v>5</v>
+      </c>
+      <c r="F18" s="7">
+        <v>10</v>
+      </c>
+      <c r="G18" s="8">
+        <v>4</v>
+      </c>
+      <c r="H18" s="17">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="I18" s="17">
+        <v>86.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="9">
+        <v>5</v>
+      </c>
+      <c r="F23" s="9">
+        <v>1</v>
+      </c>
+      <c r="G23" s="9">
+        <v>2</v>
+      </c>
+      <c r="H23" s="11">
+        <v>26.5</v>
+      </c>
+      <c r="I23" s="11">
+        <v>91.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="9">
+        <v>5</v>
+      </c>
+      <c r="F24" s="9">
+        <v>2</v>
+      </c>
+      <c r="G24" s="9">
+        <v>2</v>
+      </c>
+      <c r="H24" s="10">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="I24" s="10">
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="9">
+        <v>5</v>
+      </c>
+      <c r="F25" s="9">
+        <v>5</v>
+      </c>
+      <c r="G25" s="9">
+        <v>2</v>
+      </c>
+      <c r="H25" s="18">
+        <v>48.4</v>
+      </c>
+      <c r="I25" s="18">
+        <v>85.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="9">
+        <v>5</v>
+      </c>
+      <c r="F26" s="9">
+        <v>7</v>
+      </c>
+      <c r="G26" s="9">
+        <v>2</v>
+      </c>
+      <c r="H26" s="11">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="I26" s="11">
+        <v>89.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="9">
+        <v>5</v>
+      </c>
+      <c r="F27" s="9">
+        <v>10</v>
+      </c>
+      <c r="G27" s="9">
+        <v>2</v>
+      </c>
+      <c r="H27" s="11">
+        <v>34.1</v>
+      </c>
+      <c r="I27" s="11">
+        <v>90.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="7">
+        <v>5</v>
+      </c>
+      <c r="F29" s="7">
+        <v>1</v>
+      </c>
+      <c r="G29" s="8">
+        <v>4</v>
+      </c>
+      <c r="H29" s="16">
+        <v>33.9</v>
+      </c>
+      <c r="I29" s="16">
+        <v>92.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="7">
+        <v>5</v>
+      </c>
+      <c r="F30" s="7">
+        <v>2</v>
+      </c>
+      <c r="G30" s="8">
+        <v>4</v>
+      </c>
+      <c r="H30" s="15">
+        <v>31.3</v>
+      </c>
+      <c r="I30" s="15">
+        <v>92.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="7">
+        <v>5</v>
+      </c>
+      <c r="F31" s="7">
+        <v>5</v>
+      </c>
+      <c r="G31" s="8">
+        <v>4</v>
+      </c>
+      <c r="H31" s="12">
+        <v>28.2</v>
+      </c>
+      <c r="I31" s="12">
+        <v>94.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="7">
+        <v>5</v>
+      </c>
+      <c r="F32" s="7">
+        <v>7</v>
+      </c>
+      <c r="G32" s="8">
+        <v>4</v>
+      </c>
+      <c r="H32" s="15">
+        <v>26.9</v>
+      </c>
+      <c r="I32" s="15">
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="7">
+        <v>5</v>
+      </c>
+      <c r="F33" s="7">
+        <v>10</v>
+      </c>
+      <c r="G33" s="8">
+        <v>4</v>
+      </c>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="13">
+        <v>36.4</v>
+      </c>
+      <c r="G2" s="13">
+        <v>91.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="14">
+        <v>32.5</v>
+      </c>
+      <c r="G3" s="14">
+        <v>91.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="14">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="G4" s="14">
+        <v>92.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9">
+        <v>33.6</v>
+      </c>
+      <c r="G2" s="9">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9">
+        <v>32.5</v>
+      </c>
+      <c r="G3" s="9">
+        <v>90.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>39.1</v>
+      </c>
+      <c r="G4">
+        <v>86.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9">
+        <v>5</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2</v>
+      </c>
+      <c r="E5" s="9">
+        <v>2</v>
+      </c>
+      <c r="F5" s="9">
+        <v>39</v>
+      </c>
+      <c r="G5" s="9">
+        <v>84.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="25" customWidth="1"/>
+    <col min="11" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="28">
+        <v>17</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="J2" s="2">
+        <v>84.4</v>
+      </c>
+      <c r="K2" s="31">
+        <v>39</v>
+      </c>
+      <c r="L2" s="31">
+        <v>84.4</v>
+      </c>
+      <c r="M2">
+        <f>I2-K2</f>
+        <v>35.599999999999994</v>
+      </c>
+      <c r="N2">
+        <f>J2-L2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="28">
+        <v>17</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2">
+        <v>72</v>
+      </c>
+      <c r="J3" s="2">
+        <v>86.6</v>
+      </c>
+      <c r="K3" s="31">
+        <v>39.1</v>
+      </c>
+      <c r="L3" s="31">
+        <v>86.5</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M9" si="0">I3-K3</f>
+        <v>32.9</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N9" si="1">J3-L3</f>
+        <v>9.9999999999994316E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="28">
+        <v>17</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="2">
+        <v>61.2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>90.1</v>
+      </c>
+      <c r="K4" s="32">
+        <v>32.5</v>
+      </c>
+      <c r="L4" s="32">
+        <v>90.2</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>28.700000000000003</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>-0.10000000000000853</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="28">
+        <v>17</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="2">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="J5" s="2">
+        <v>90.3</v>
+      </c>
+      <c r="K5" s="31">
+        <v>39.9</v>
+      </c>
+      <c r="L5" s="31">
+        <v>90.3</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>26.000000000000007</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="28">
+        <v>17</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="21">
+        <v>1</v>
+      </c>
+      <c r="E6" s="21">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21">
+        <v>5</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="2">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="J6" s="2">
+        <v>91.8</v>
+      </c>
+      <c r="K6" s="31">
+        <v>32.6</v>
+      </c>
+      <c r="L6" s="31">
+        <v>92</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>32.300000000000004</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>-0.20000000000000284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="28">
+        <v>17</v>
+      </c>
+      <c r="B7" s="29">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2</v>
+      </c>
+      <c r="H7" s="5">
+        <v>15</v>
+      </c>
+      <c r="I7" s="2">
+        <v>74.7</v>
+      </c>
+      <c r="J7" s="2">
+        <v>84.1</v>
+      </c>
+      <c r="K7" s="31">
+        <v>53</v>
+      </c>
+      <c r="L7" s="31">
+        <v>84</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>21.700000000000003</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>9.9999999999994316E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="28">
+        <v>17</v>
+      </c>
+      <c r="B8" s="29">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>15</v>
+      </c>
+      <c r="I8" s="2">
+        <v>77.3</v>
+      </c>
+      <c r="J8" s="2">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="K8" s="31">
+        <v>65.7</v>
+      </c>
+      <c r="L8" s="31">
+        <v>72.5</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>11.599999999999994</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>9.9999999999994316E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="28">
+        <v>17</v>
+      </c>
+      <c r="B9" s="29">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>5</v>
+      </c>
+      <c r="G9" s="5">
+        <v>5</v>
+      </c>
+      <c r="H9" s="5">
+        <v>15</v>
+      </c>
+      <c r="I9" s="27">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="J9" s="27">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="K9" s="33">
+        <v>61.5</v>
+      </c>
+      <c r="L9" s="33">
+        <v>80.5</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>12.099999999999994</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>9.9999999999994316E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="28">
+        <v>17</v>
+      </c>
+      <c r="B10" s="30">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working on general CRNN architecture
</commit_message>
<xml_diff>
--- a/Writeups/Experiments.xlsx
+++ b/Writeups/Experiments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Fuzzy Boundary Exp" sheetId="1" r:id="rId1"/>
@@ -493,7 +493,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -684,11 +683,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1803424160"/>
-        <c:axId val="1803354608"/>
+        <c:axId val="137423216"/>
+        <c:axId val="137427568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1803424160"/>
+        <c:axId val="137423216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -744,12 +743,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1803354608"/>
+        <c:crossAx val="137427568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1803354608"/>
+        <c:axId val="137427568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -805,7 +804,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1803424160"/>
+        <c:crossAx val="137423216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2704,7 +2703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="H8" sqref="H8:I8"/>
     </sheetView>
   </sheetViews>
@@ -3035,7 +3034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView zoomScale="98" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added larger call windows to testing
</commit_message>
<xml_diff>
--- a/Writeups/Experiments.xlsx
+++ b/Writeups/Experiments.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathangomesselman/Documents/Research/ElephantCallAI/Writeups/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E72DC32-9100-1D40-949B-3DA9BB67E9DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fuzzy Boundary Exp" sheetId="1" r:id="rId1"/>
@@ -17,11 +18,14 @@
     <sheet name="Combined Number" sheetId="9" r:id="rId3"/>
     <sheet name="Hierarchical Exp" sheetId="5" r:id="rId4"/>
     <sheet name="Negative Factor Exp" sheetId="3" r:id="rId5"/>
-    <sheet name="Cuda SEED" sheetId="6" r:id="rId6"/>
-    <sheet name="Shift Window" sheetId="7" r:id="rId7"/>
-    <sheet name="No nn04d_20181030" sheetId="8" r:id="rId8"/>
+    <sheet name="Repeatability" sheetId="11" r:id="rId6"/>
+    <sheet name="Cuda SEED" sheetId="6" r:id="rId7"/>
+    <sheet name="Shift Window" sheetId="7" r:id="rId8"/>
+    <sheet name="No nn04d_20181030" sheetId="8" r:id="rId9"/>
+    <sheet name="Eval_Params" sheetId="13" r:id="rId10"/>
+    <sheet name="Bai" sheetId="14" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="71">
   <si>
     <t>Fuzzy Boundary</t>
   </si>
@@ -202,12 +206,57 @@
   </si>
   <si>
     <t>Subsample Data P/R</t>
+  </si>
+  <si>
+    <t>Number of Shuffles</t>
+  </si>
+  <si>
+    <t>Val R</t>
+  </si>
+  <si>
+    <t>Val P</t>
+  </si>
+  <si>
+    <t>Val Acc</t>
+  </si>
+  <si>
+    <t>Val F1</t>
+  </si>
+  <si>
+    <t>OLD INIT WITH SHUFFLE</t>
+  </si>
+  <si>
+    <t>Min Call Length</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>FULL F1</t>
+  </si>
+  <si>
+    <t>Slide % overlap</t>
+  </si>
+  <si>
+    <t>Train Type</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Solo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 0 </t>
+  </si>
+  <si>
+    <t>Model 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -258,7 +307,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,8 +338,68 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -383,8 +492,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -406,8 +528,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -444,8 +568,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -456,6 +594,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -466,20 +605,30 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5500"/>
+      <color rgb="FFDC1F21"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -560,19 +709,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.600000000000001</c:v>
+                  <c:v>1.6000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.600000000000001</c:v>
+                  <c:v>1.6000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.100000000000001</c:v>
+                  <c:v>5.1000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-0.5</c:v>
@@ -581,34 +730,34 @@
                   <c:v>-2.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.200000000000003</c:v>
+                  <c:v>0.20000000000000284</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.400000000000002</c:v>
+                  <c:v>1.4000000000000021</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.399999999999999</c:v>
+                  <c:v>-0.39999999999999858</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.900000000000002</c:v>
+                  <c:v>0.90000000000000213</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.800000000000001</c:v>
+                  <c:v>3.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.400000000000002</c:v>
+                  <c:v>1.4000000000000021</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.200000000000003</c:v>
+                  <c:v>3.2000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -620,60 +769,65 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.200000000000003</c:v>
+                  <c:v>1.2000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.700000000000003</c:v>
+                  <c:v>1.7000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.299999999999997</c:v>
+                  <c:v>-3.2999999999999972</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.900000000000006</c:v>
+                  <c:v>2.9000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.200000000000003</c:v>
+                  <c:v>1.2000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.200000000000003</c:v>
+                  <c:v>2.2000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.200000000000003</c:v>
+                  <c:v>1.2000000000000028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0747-2640-AF2E-F0B9C6322EFA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -683,11 +837,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137423216"/>
-        <c:axId val="137427568"/>
+        <c:axId val="-237057408"/>
+        <c:axId val="-237053248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137423216"/>
+        <c:axId val="-237057408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -707,6 +861,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -743,12 +898,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137427568"/>
+        <c:crossAx val="-237053248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137427568"/>
+        <c:axId val="-237053248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -768,6 +923,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -804,7 +960,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137423216"/>
+        <c:crossAx val="-237057408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1426,7 +1582,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1706,11 +1868,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:F21"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2275,12 +2437,687 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="39">
+        <v>15</v>
+      </c>
+      <c r="F2" s="40">
+        <v>15</v>
+      </c>
+      <c r="G2" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="46">
+        <v>70.3</v>
+      </c>
+      <c r="J2" s="46">
+        <v>77</v>
+      </c>
+      <c r="K2" s="46">
+        <v>73.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="39">
+        <v>15</v>
+      </c>
+      <c r="F3" s="40">
+        <v>15</v>
+      </c>
+      <c r="G3" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="39">
+        <v>0.75</v>
+      </c>
+      <c r="I3" s="46">
+        <v>74.3</v>
+      </c>
+      <c r="J3" s="46">
+        <v>73.7</v>
+      </c>
+      <c r="K3" s="46">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="39">
+        <v>15</v>
+      </c>
+      <c r="F4" s="40">
+        <v>15</v>
+      </c>
+      <c r="G4" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="39">
+        <v>0.85</v>
+      </c>
+      <c r="I4" s="46">
+        <v>77.2</v>
+      </c>
+      <c r="J4" s="46">
+        <v>71.7</v>
+      </c>
+      <c r="K4" s="46">
+        <v>74.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="39">
+        <v>15</v>
+      </c>
+      <c r="F5" s="40">
+        <v>15</v>
+      </c>
+      <c r="G5" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="39">
+        <v>0.95</v>
+      </c>
+      <c r="I5" s="46">
+        <v>83.8</v>
+      </c>
+      <c r="J5" s="46">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="K5" s="46">
+        <v>73.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="39">
+        <v>15</v>
+      </c>
+      <c r="F6" s="43">
+        <v>10</v>
+      </c>
+      <c r="G6" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="45">
+        <v>62.5</v>
+      </c>
+      <c r="J6" s="45">
+        <v>80.2</v>
+      </c>
+      <c r="K6" s="45">
+        <v>70.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="39">
+        <v>15</v>
+      </c>
+      <c r="F7" s="43">
+        <v>10</v>
+      </c>
+      <c r="G7" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="44">
+        <v>0.75</v>
+      </c>
+      <c r="I7" s="45">
+        <v>70.5</v>
+      </c>
+      <c r="J7" s="45">
+        <v>76.7</v>
+      </c>
+      <c r="K7" s="45">
+        <v>73.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="39">
+        <v>15</v>
+      </c>
+      <c r="F8" s="43">
+        <v>10</v>
+      </c>
+      <c r="G8" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="44">
+        <v>0.85</v>
+      </c>
+      <c r="I8" s="45">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="J8" s="45">
+        <v>75</v>
+      </c>
+      <c r="K8" s="45">
+        <v>74.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="39">
+        <v>15</v>
+      </c>
+      <c r="F9" s="43">
+        <v>10</v>
+      </c>
+      <c r="G9" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="44">
+        <v>0.95</v>
+      </c>
+      <c r="I9" s="45">
+        <v>79.2</v>
+      </c>
+      <c r="J9" s="45">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="K9" s="45">
+        <v>75.400000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="39">
+        <v>15</v>
+      </c>
+      <c r="F11" s="40">
+        <v>15</v>
+      </c>
+      <c r="G11" s="42">
+        <v>0.75</v>
+      </c>
+      <c r="H11" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="46">
+        <v>71</v>
+      </c>
+      <c r="J11" s="46">
+        <v>77.7</v>
+      </c>
+      <c r="K11" s="46">
+        <v>74.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="39">
+        <v>15</v>
+      </c>
+      <c r="F12" s="40">
+        <v>15</v>
+      </c>
+      <c r="G12" s="42">
+        <v>0.75</v>
+      </c>
+      <c r="H12" s="39">
+        <v>0.75</v>
+      </c>
+      <c r="I12" s="46">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="J12" s="46">
+        <v>73.5</v>
+      </c>
+      <c r="K12" s="46">
+        <v>74.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="39">
+        <v>15</v>
+      </c>
+      <c r="F13" s="40">
+        <v>15</v>
+      </c>
+      <c r="G13" s="42">
+        <v>0.75</v>
+      </c>
+      <c r="H13" s="39">
+        <v>0.85</v>
+      </c>
+      <c r="I13" s="46">
+        <v>79.2</v>
+      </c>
+      <c r="J13" s="46">
+        <v>71.2</v>
+      </c>
+      <c r="K13" s="46">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="39">
+        <v>15</v>
+      </c>
+      <c r="F14" s="40">
+        <v>15</v>
+      </c>
+      <c r="G14" s="42">
+        <v>0.75</v>
+      </c>
+      <c r="H14" s="39">
+        <v>0.95</v>
+      </c>
+      <c r="I14" s="46">
+        <v>84.6</v>
+      </c>
+      <c r="J14" s="46">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="K14" s="46">
+        <v>74.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="39">
+        <v>15</v>
+      </c>
+      <c r="F15" s="47">
+        <v>10</v>
+      </c>
+      <c r="G15" s="42">
+        <v>0.75</v>
+      </c>
+      <c r="H15" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="49">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="J15" s="49">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="K15" s="49">
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="39">
+        <v>15</v>
+      </c>
+      <c r="F16" s="47">
+        <v>10</v>
+      </c>
+      <c r="G16" s="42">
+        <v>0.75</v>
+      </c>
+      <c r="H16" s="48">
+        <v>0.75</v>
+      </c>
+      <c r="I16" s="49">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="J16" s="49">
+        <v>77.7</v>
+      </c>
+      <c r="K16" s="49">
+        <v>74.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="39">
+        <v>15</v>
+      </c>
+      <c r="F17" s="47">
+        <v>10</v>
+      </c>
+      <c r="G17" s="42">
+        <v>0.75</v>
+      </c>
+      <c r="H17" s="48">
+        <v>0.85</v>
+      </c>
+      <c r="I17" s="49">
+        <v>74.3</v>
+      </c>
+      <c r="J17" s="49">
+        <v>74.5</v>
+      </c>
+      <c r="K17" s="49">
+        <v>74.400000000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="39">
+        <v>15</v>
+      </c>
+      <c r="F18" s="47">
+        <v>10</v>
+      </c>
+      <c r="G18" s="42">
+        <v>0.75</v>
+      </c>
+      <c r="H18" s="48">
+        <v>0.95</v>
+      </c>
+      <c r="I18" s="49">
+        <v>80.5</v>
+      </c>
+      <c r="J18" s="49">
+        <v>70.7</v>
+      </c>
+      <c r="K18" s="49">
+        <v>75.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5BA505-BDFA-0E4E-A9FA-CD25260EC55D}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J5" sqref="I5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2649,7 +3486,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2700,11 +3537,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:I8"/>
+      <selection activeCell="C1" sqref="C1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3031,11 +3868,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F33"/>
+    <sheetView zoomScale="98" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4051,7 +4888,458 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3">
+        <v>97.9</v>
+      </c>
+      <c r="G2" s="5">
+        <v>87.7</v>
+      </c>
+      <c r="H2" s="3">
+        <v>87.8</v>
+      </c>
+      <c r="I2" s="3">
+        <v>87.5</v>
+      </c>
+      <c r="J2" s="3">
+        <v>43.3</v>
+      </c>
+      <c r="K2" s="3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3">
+        <v>97.9</v>
+      </c>
+      <c r="G3" s="3">
+        <v>87.8</v>
+      </c>
+      <c r="H3" s="3">
+        <v>86.4</v>
+      </c>
+      <c r="I3" s="3">
+        <v>89.3</v>
+      </c>
+      <c r="J3" s="3">
+        <v>41.9</v>
+      </c>
+      <c r="K3" s="3">
+        <v>86.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3">
+        <v>98</v>
+      </c>
+      <c r="G4" s="3">
+        <v>88</v>
+      </c>
+      <c r="H4" s="3">
+        <v>89</v>
+      </c>
+      <c r="I4" s="3">
+        <v>87</v>
+      </c>
+      <c r="J4" s="3">
+        <v>42.4</v>
+      </c>
+      <c r="K4" s="3">
+        <v>84.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3">
+        <v>97.9</v>
+      </c>
+      <c r="G5" s="3">
+        <v>87.3</v>
+      </c>
+      <c r="H5" s="3">
+        <v>88.7</v>
+      </c>
+      <c r="I5" s="3">
+        <v>86</v>
+      </c>
+      <c r="J5" s="3">
+        <v>36.9</v>
+      </c>
+      <c r="K5" s="3">
+        <v>88.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3">
+        <v>97.9</v>
+      </c>
+      <c r="G6" s="3">
+        <v>97.2</v>
+      </c>
+      <c r="H6" s="3">
+        <v>89.7</v>
+      </c>
+      <c r="I6" s="3">
+        <v>84.8</v>
+      </c>
+      <c r="J6" s="3">
+        <v>32.1</v>
+      </c>
+      <c r="K6" s="3">
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3">
+        <v>97.9</v>
+      </c>
+      <c r="G9" s="3">
+        <v>87.7</v>
+      </c>
+      <c r="H9" s="3">
+        <v>87.2</v>
+      </c>
+      <c r="I9" s="3">
+        <v>88.3</v>
+      </c>
+      <c r="J9" s="3">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="K9" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>10</v>
+      </c>
+      <c r="F10" s="3">
+        <v>98</v>
+      </c>
+      <c r="G10" s="3">
+        <v>87.9</v>
+      </c>
+      <c r="H10" s="3">
+        <v>90.2</v>
+      </c>
+      <c r="I10" s="3">
+        <v>85.8</v>
+      </c>
+      <c r="J10" s="3">
+        <v>36.9</v>
+      </c>
+      <c r="K10" s="3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5">
+        <v>10</v>
+      </c>
+      <c r="F11" s="3">
+        <v>97.8</v>
+      </c>
+      <c r="G11" s="3">
+        <v>86.9</v>
+      </c>
+      <c r="H11" s="3">
+        <v>87.4</v>
+      </c>
+      <c r="I11" s="3">
+        <v>86.5</v>
+      </c>
+      <c r="J11" s="3">
+        <v>42</v>
+      </c>
+      <c r="K11" s="3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" s="5">
+        <v>10</v>
+      </c>
+      <c r="F12" s="5">
+        <v>97.9</v>
+      </c>
+      <c r="G12" s="5">
+        <v>87.6</v>
+      </c>
+      <c r="H12" s="5">
+        <v>88</v>
+      </c>
+      <c r="I12" s="5">
+        <v>87.2</v>
+      </c>
+      <c r="J12" s="3">
+        <v>35.4</v>
+      </c>
+      <c r="K12" s="3">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5">
+        <v>97.8</v>
+      </c>
+      <c r="G13" s="5">
+        <v>86.9</v>
+      </c>
+      <c r="H13" s="5">
+        <v>89.2</v>
+      </c>
+      <c r="I13" s="5">
+        <v>84.7</v>
+      </c>
+      <c r="J13" s="3">
+        <v>30.1</v>
+      </c>
+      <c r="K13" s="3">
+        <v>90.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+      <c r="E14" s="5">
+        <v>10</v>
+      </c>
+      <c r="F14" s="5">
+        <v>97.9</v>
+      </c>
+      <c r="G14" s="5">
+        <v>87.7</v>
+      </c>
+      <c r="H14" s="5">
+        <v>87.4</v>
+      </c>
+      <c r="I14" s="5">
+        <v>87.9</v>
+      </c>
+      <c r="J14" s="5">
+        <v>33.4</v>
+      </c>
+      <c r="K14" s="5">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4162,8 +5450,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
@@ -4299,8 +5587,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>